<commit_message>
Ya funcionan las distancias, queda mejorar el modelo
</commit_message>
<xml_diff>
--- a/planos/comprobar_manual/results_final/10_sensors.xlsx
+++ b/planos/comprobar_manual/results_final/10_sensors.xlsx
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3.022884460504618</v>
+        <v>3.015327856792667</v>
       </c>
       <c r="F2" t="n">
-        <v>1.91345426272993</v>
+        <v>1.908671011575838</v>
       </c>
       <c r="G2" t="n">
         <v>0.1</v>
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>7.217892821295916</v>
+        <v>7.199849539655979</v>
       </c>
       <c r="F3" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G3" t="n">
         <v>0.1</v>
@@ -554,10 +554,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>7.217892821295916</v>
+        <v>7.199849539655979</v>
       </c>
       <c r="F4" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G4" t="n">
         <v>0.6</v>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>7.217892821295916</v>
+        <v>7.199849539655979</v>
       </c>
       <c r="F5" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -616,10 +616,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7.217892821295916</v>
+        <v>7.199849539655979</v>
       </c>
       <c r="F6" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G6" t="n">
         <v>1.1</v>
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>9.652482235983669</v>
+        <v>9.628352970030249</v>
       </c>
       <c r="F7" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G7" t="n">
         <v>0.1</v>
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>9.652482235983669</v>
+        <v>9.628352970030249</v>
       </c>
       <c r="F8" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G8" t="n">
         <v>0.6</v>
@@ -709,10 +709,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>9.652482235983669</v>
+        <v>9.628352970030249</v>
       </c>
       <c r="F9" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -740,10 +740,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>9.652482235983669</v>
+        <v>9.628352970030249</v>
       </c>
       <c r="F10" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G10" t="n">
         <v>1.1</v>
@@ -771,10 +771,10 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F11" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G11" t="n">
         <v>0.1</v>
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F12" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G12" t="n">
         <v>1.1</v>
@@ -833,10 +833,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F13" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G13" t="n">
         <v>1.7</v>
@@ -864,10 +864,10 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F14" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G14" t="n">
         <v>1.1</v>
@@ -895,10 +895,10 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F15" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G15" t="n">
         <v>1.1</v>
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8.435187528639792</v>
+        <v>8.414101254843114</v>
       </c>
       <c r="F16" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -957,10 +957,10 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>12.08707165067142</v>
+        <v>12.05685640040452</v>
       </c>
       <c r="F17" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G17" t="n">
         <v>0.1</v>
@@ -988,10 +988,10 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>12.08707165067142</v>
+        <v>12.05685640040452</v>
       </c>
       <c r="F18" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G18" t="n">
         <v>0.6</v>
@@ -1019,10 +1019,10 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>12.08707165067142</v>
+        <v>12.05685640040452</v>
       </c>
       <c r="F19" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -1050,10 +1050,10 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>12.08707165067142</v>
+        <v>12.05685640040452</v>
       </c>
       <c r="F20" t="n">
-        <v>2.736018428901923</v>
+        <v>2.729178932624134</v>
       </c>
       <c r="G20" t="n">
         <v>1.1</v>
@@ -1081,10 +1081,10 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>14.52166106535918</v>
+        <v>14.48535983077879</v>
       </c>
       <c r="F21" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G21" t="n">
         <v>0.1</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>14.52166106535918</v>
+        <v>14.48535983077879</v>
       </c>
       <c r="F22" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G22" t="n">
         <v>0.6</v>
@@ -1143,10 +1143,10 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>14.52166106535918</v>
+        <v>14.48535983077879</v>
       </c>
       <c r="F23" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -1174,10 +1174,10 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>14.52166106535918</v>
+        <v>14.48535983077879</v>
       </c>
       <c r="F24" t="n">
-        <v>1.038111679226371</v>
+        <v>1.035516608633646</v>
       </c>
       <c r="G24" t="n">
         <v>1.1</v>
@@ -1205,10 +1205,10 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F25" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G25" t="n">
         <v>0.1</v>
@@ -1236,10 +1236,10 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F26" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G26" t="n">
         <v>1.1</v>
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F27" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G27" t="n">
         <v>1.7</v>
@@ -1298,10 +1298,10 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F28" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G28" t="n">
         <v>1.1</v>
@@ -1329,10 +1329,10 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F29" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G29" t="n">
         <v>1.1</v>
@@ -1360,10 +1360,10 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>13.3043663580153</v>
+        <v>13.27110811559165</v>
       </c>
       <c r="F30" t="n">
-        <v>1.887065054064147</v>
+        <v>1.88234777062889</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1391,10 +1391,10 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>18.35517791337526</v>
+        <v>18.30929365700822</v>
       </c>
       <c r="F31" t="n">
-        <v>2.742532139958338</v>
+        <v>2.735676360711819</v>
       </c>
       <c r="G31" t="n">
         <v>0.1</v>
@@ -1422,10 +1422,10 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>18.35517791337526</v>
+        <v>18.30929365700822</v>
       </c>
       <c r="F32" t="n">
-        <v>2.742532139958338</v>
+        <v>2.735676360711819</v>
       </c>
       <c r="G32" t="n">
         <v>0.6</v>
@@ -1453,10 +1453,10 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>18.35517791337526</v>
+        <v>18.30929365700822</v>
       </c>
       <c r="F33" t="n">
-        <v>2.742532139958338</v>
+        <v>2.735676360711819</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>18.35517791337526</v>
+        <v>18.30929365700822</v>
       </c>
       <c r="F34" t="n">
-        <v>2.742532139958338</v>
+        <v>2.735676360711819</v>
       </c>
       <c r="G34" t="n">
         <v>1.1</v>
@@ -1515,10 +1515,10 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>20.59522134803255</v>
+        <v>20.54373743320868</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9847383194132995</v>
+        <v>0.9822766714948948</v>
       </c>
       <c r="G35" t="n">
         <v>0.1</v>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>20.59522134803255</v>
+        <v>20.54373743320868</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9847383194132995</v>
+        <v>0.9822766714948948</v>
       </c>
       <c r="G36" t="n">
         <v>0.6</v>
@@ -1577,10 +1577,10 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>20.59522134803255</v>
+        <v>20.54373743320868</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9847383194132995</v>
+        <v>0.9822766714948948</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
@@ -1608,10 +1608,10 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>20.59522134803255</v>
+        <v>20.54373743320868</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9847383194132995</v>
+        <v>0.9822766714948948</v>
       </c>
       <c r="G38" t="n">
         <v>1.1</v>
@@ -1639,10 +1639,10 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F39" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G39" t="n">
         <v>0.1</v>
@@ -1670,10 +1670,10 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F40" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G40" t="n">
         <v>1.1</v>
@@ -1701,10 +1701,10 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F41" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G41" t="n">
         <v>1.7</v>
@@ -1732,10 +1732,10 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F42" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G42" t="n">
         <v>1.1</v>
@@ -1763,10 +1763,10 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F43" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G43" t="n">
         <v>1.1</v>
@@ -1794,10 +1794,10 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>19.47519963070391</v>
+        <v>19.42651554510845</v>
       </c>
       <c r="F44" t="n">
-        <v>1.863635229685819</v>
+        <v>1.858976516103357</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1825,10 +1825,10 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>16.32223366053932</v>
+        <v>16.28143135629049</v>
       </c>
       <c r="F45" t="n">
-        <v>1.866451058200372</v>
+        <v>1.861785305612455</v>
       </c>
       <c r="G45" t="n">
         <v>0.1</v>
@@ -1856,10 +1856,10 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>16.32223366053932</v>
+        <v>16.28143135629049</v>
       </c>
       <c r="F46" t="n">
-        <v>1.866451058200372</v>
+        <v>1.861785305612455</v>
       </c>
       <c r="G46" t="n">
         <v>1.7</v>
@@ -1887,10 +1887,10 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>21.93261821888514</v>
+        <v>21.87779108062992</v>
       </c>
       <c r="F47" t="n">
-        <v>1.863658697566219</v>
+        <v>1.858999925318772</v>
       </c>
       <c r="G47" t="n">
         <v>0.1</v>
@@ -1918,10 +1918,10 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>21.93261821888514</v>
+        <v>21.87779108062992</v>
       </c>
       <c r="F48" t="n">
-        <v>1.863658697566219</v>
+        <v>1.858999925318772</v>
       </c>
       <c r="G48" t="n">
         <v>1.1</v>
@@ -1949,10 +1949,10 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>21.93261821888514</v>
+        <v>21.87779108062992</v>
       </c>
       <c r="F49" t="n">
-        <v>1.863658697566219</v>
+        <v>1.858999925318772</v>
       </c>
       <c r="G49" t="n">
         <v>1.7</v>
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>21.93261821888514</v>
+        <v>21.87779108062992</v>
       </c>
       <c r="F50" t="n">
-        <v>1.863658697566219</v>
+        <v>1.858999925318772</v>
       </c>
       <c r="G50" t="n">
         <v>1.1</v>

</xml_diff>